<commit_message>
edit readme and add new.md
</commit_message>
<xml_diff>
--- a/resources/TestData.xlsx
+++ b/resources/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4C1894-84C1-4F6A-A2FA-8E1365FC2FB6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB4A4C6-D265-40E1-A4DC-44414645483E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
     <t>SearchItem</t>
   </si>
   <si>
-    <t>Sumsang a50 mobile phone</t>
+    <t>Sumsang a50s mobile phone</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>